<commit_message>
Updated all test documents added test percentage
</commit_message>
<xml_diff>
--- a/documentation/quality/Test Documents/01 TC - Log In.Index.xlsx
+++ b/documentation/quality/Test Documents/01 TC - Log In.Index.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="19440" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="136">
   <si>
     <t>Tester:</t>
   </si>
@@ -507,12 +507,42 @@
       <t xml:space="preserve"> as part of the High priority testing requirements.</t>
     </r>
   </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>not run</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>blocked</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,7 +584,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,6 +600,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -766,6 +808,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,6 +944,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -956,6 +1027,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -990,6 +1062,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1165,14 +1238,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:O7"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -1180,9 +1253,10 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>123</v>
       </c>
@@ -1193,7 +1267,7 @@
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -1203,8 +1277,23 @@
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
       <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="I2" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
@@ -1214,8 +1303,28 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="I3" s="40">
+        <f>AVERAGE(Sheet2!B12/38)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="40">
+        <f>AVERAGE(Sheet2!C12/38)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="40">
+        <f>AVERAGE(Sheet2!D12/38)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="40">
+        <f>AVERAGE(Sheet2!E12/38)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="40">
+        <f>SUM(I3:L4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>124</v>
       </c>
@@ -1225,8 +1334,13 @@
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
       <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1239,7 +1353,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1262,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="120.75" thickBot="1">
+    <row r="7" spans="1:15" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1288,7 +1402,7 @@
       <c r="N7" s="28"/>
       <c r="O7" s="29"/>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1305,7 +1419,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="120">
+    <row r="9" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1322,7 +1436,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="45">
+    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1453,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="45">
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1470,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="45">
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1373,7 +1487,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="60">
+    <row r="13" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1390,7 +1504,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -1403,7 +1517,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="45">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1420,7 +1534,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="45">
+    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -1437,7 +1551,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="45">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
@@ -1454,7 +1568,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="45">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -1473,7 +1587,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="30">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1492,7 +1606,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="45">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>41</v>
       </c>
@@ -1509,7 +1623,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>2</v>
       </c>
@@ -1522,7 +1636,7 @@
       <c r="F21" s="13"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="120">
+    <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1539,7 +1653,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="345">
+    <row r="23" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
@@ -1556,7 +1670,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
@@ -1573,7 +1687,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="30">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
@@ -1590,7 +1704,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
@@ -1607,7 +1721,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
@@ -1624,7 +1738,7 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="45">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>61</v>
       </c>
@@ -1641,7 +1755,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>72</v>
       </c>
@@ -1658,7 +1772,7 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
@@ -1675,7 +1789,7 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="30">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>74</v>
       </c>
@@ -1692,7 +1806,7 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="45">
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
@@ -1709,7 +1823,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="30">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
@@ -1726,7 +1840,7 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="30">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>2.1</v>
       </c>
@@ -1739,7 +1853,7 @@
       <c r="F34" s="13"/>
       <c r="G34" s="19"/>
     </row>
-    <row r="35" spans="1:7" ht="45">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
@@ -1756,7 +1870,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="45">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>92</v>
       </c>
@@ -1773,7 +1887,7 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="60">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>93</v>
       </c>
@@ -1790,7 +1904,7 @@
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="45">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>94</v>
       </c>
@@ -1807,7 +1921,7 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="45">
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
@@ -1824,7 +1938,7 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="45">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
@@ -1841,7 +1955,7 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="45">
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>97</v>
       </c>
@@ -1858,7 +1972,7 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="60">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>108</v>
       </c>
@@ -1875,7 +1989,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="45">
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>109</v>
       </c>
@@ -1892,7 +2006,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="45">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>110</v>
       </c>
@@ -1909,7 +2023,7 @@
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="45">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>116</v>
       </c>
@@ -1926,7 +2040,7 @@
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="30">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>117</v>
       </c>
@@ -1943,7 +2057,7 @@
       </c>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="45.75" thickBot="1">
+    <row r="47" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>118</v>
       </c>
@@ -1962,33 +2076,38 @@
       </c>
       <c r="G47" s="18"/>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="319" spans="1:1">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="320" spans="1:1">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <conditionalFormatting sqref="F7">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="BLOCKED">
@@ -2056,33 +2175,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="39">
+        <v>1</v>
+      </c>
+      <c r="B8" s="33">
+        <f>COUNTIF(Sheet1!F7:F13, "PASS")</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="33">
+        <f>COUNTIF(Sheet1!F7:F13, "FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <f>COUNTIF(Sheet1!F7:F13, "NOT RUN")</f>
+        <v>7</v>
+      </c>
+      <c r="E8" s="33">
+        <f>COUNTIF(Sheet1!F7:F13, "BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B9" s="33">
+        <f>COUNTIF(Sheet1!F15:F20, "PASS")</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="33">
+        <f>COUNTIF(Sheet1!F15:F20, "FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <f>COUNTIF(Sheet1!F15:F20, "NOT RUN")</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="33">
+        <f>COUNTIF(Sheet1!F15:F20, "BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="39">
+        <v>2</v>
+      </c>
+      <c r="B10" s="33">
+        <f>COUNTIF(Sheet1!F22:F33, "PASS")</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="33">
+        <f>COUNTIF(Sheet1!F22:F33, "FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <f>COUNTIF(Sheet1!F22:F33, "NOT RUN")</f>
+        <v>12</v>
+      </c>
+      <c r="E10" s="33">
+        <f>COUNTIF(Sheet1!F22:F33, "BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="39">
+        <v>2.1</v>
+      </c>
+      <c r="B11" s="33">
+        <f>COUNTIF(Sheet1!F35:F47, "PASS")</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="33">
+        <f>COUNTIF(Sheet1!F35:F47, "FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <f>COUNTIF(Sheet1!F35:F47, "NOT RUN")</f>
+        <v>13</v>
+      </c>
+      <c r="E11" s="33">
+        <f>COUNTIF(Sheet1!F35:F47, "BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B8:B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C8:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>SUM(D8:D11)</f>
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2091,31 +2335,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Reverted previous button placement in customer/index.php
</commit_message>
<xml_diff>
--- a/documentation/quality/Test Documents/01 TC - Log In.Index.xlsx
+++ b/documentation/quality/Test Documents/01 TC - Log In.Index.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="19440" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="135">
   <si>
     <t>Tester:</t>
   </si>
@@ -73,17 +73,9 @@
     <t>Resources for the Blind, Inc Logo</t>
   </si>
   <si>
-    <t>RBI Logo should be present</t>
-  </si>
-  <si>
     <t>UITC_LI03</t>
   </si>
   <si>
-    <t>The following labels should be present:
-Login
-Please fill out  the following fields to login</t>
-  </si>
-  <si>
     <t>UITC_LI04</t>
   </si>
   <si>
@@ -96,46 +88,24 @@
     <t>Username textbox field</t>
   </si>
   <si>
-    <t>Username textbox field should be present</t>
-  </si>
-  <si>
-    <t>Password textbox field should be present</t>
-  </si>
-  <si>
     <t>UITC_LI06</t>
   </si>
   <si>
     <t>Remember me checkbox</t>
   </si>
   <si>
-    <t>Checkbox named Remember me should be present</t>
-  </si>
-  <si>
     <t>UITC_LI07</t>
   </si>
   <si>
     <t>Log in Button</t>
   </si>
   <si>
-    <t>Button label: Log in
-Button color: Blue</t>
-  </si>
-  <si>
     <t>FTC_LI01</t>
   </si>
   <si>
     <t>Log in - Functionality</t>
   </si>
   <si>
-    <t xml:space="preserve">Header color: Blue
-Font color: White
-Links present: 
-RBI Inventory System
-Inventory
-Log In
-</t>
-  </si>
-  <si>
     <t>Should be redirected to the Log in page</t>
   </si>
   <si>
@@ -151,9 +121,6 @@
     <t>FTC_LI05</t>
   </si>
   <si>
-    <t>FTC_LI06</t>
-  </si>
-  <si>
     <t>Click RBI Inventory System link in the Navigation bar</t>
   </si>
   <si>
@@ -166,18 +133,9 @@
     <t>Input username on username textbox field</t>
   </si>
   <si>
-    <t>Username input should appear</t>
-  </si>
-  <si>
     <t>Username: rbiadmin</t>
   </si>
   <si>
-    <t>Password input should appear</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Input password on password textbox field</t>
   </si>
   <si>
@@ -191,15 +149,6 @@
   </si>
   <si>
     <t>UITC_IP01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Header color: Blue
-Font color: White
-Links present: 
-RBI Inventory System
-Inventory
-Logout(rbiadmin)
-</t>
   </si>
   <si>
     <t>UITC_IP02</t>
@@ -537,12 +486,103 @@
   <si>
     <t>total</t>
   </si>
+  <si>
+    <t>Password: rbiadmin</t>
+  </si>
+  <si>
+    <t>Header color: Blue
+Font color: White
+Links present: 
+RBI Inventory System
+Log In (Highlighted Green)
+Should be able to hear:
+Log In
+RBI Inventory System</t>
+  </si>
+  <si>
+    <t>RBI Logo should be present
+Should be able to hear:
+Graphic RBI Logo</t>
+  </si>
+  <si>
+    <t>The following labels should be present and heard:
+Login
+Please fill out  the following fields to login</t>
+  </si>
+  <si>
+    <t>Username textbox field should be present
+Should be able to hear:
+Username
+Edit</t>
+  </si>
+  <si>
+    <t>Password textbox field should be present
+Should be able to hear:
+Password
+Edit protected</t>
+  </si>
+  <si>
+    <t>Button label: Log in
+Button color: Blue
+Should be able to hear:
+Button Login</t>
+  </si>
+  <si>
+    <t>Checkbox named Remember me should be present
+Should be able to hear:
+Checkbox checked Remember me</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Username input should appear
+Should be able to hear:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>per letter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Password input should appear
+Should be able to hear:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>star (***)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Header color: Blue
+Font color: White
+Links present: 
+RBI Inventory System
+Customer
+Logout(rbiadmin)
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,20 +834,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -829,6 +855,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -836,49 +876,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1027,7 +1025,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1062,7 +1059,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1238,14 +1234,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O320"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -1256,53 +1252,53 @@
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="I2" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
+      <c r="I2" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
       <c r="I3" s="40">
         <f>AVERAGE(Sheet2!B12/38)</f>
         <v>0</v>
@@ -1313,7 +1309,7 @@
       </c>
       <c r="K3" s="40">
         <f>AVERAGE(Sheet2!D12/38)</f>
-        <v>1</v>
+        <v>0.97368421052631582</v>
       </c>
       <c r="L3" s="40">
         <f>AVERAGE(Sheet2!E12/38)</f>
@@ -1321,26 +1317,26 @@
       </c>
       <c r="M3" s="40">
         <f>SUM(I3:L4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
+        <v>0.97368421052631582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
       <c r="I4" s="40"/>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
       <c r="M4" s="40"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1353,7 +1349,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="A6" s="20" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="210.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1384,7 +1380,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1392,17 +1388,17 @@
         <v>9</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="I7" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I7" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="36"/>
+    </row>
+    <row r="8" spans="1:15" ht="90">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1410,7 +1406,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1419,15 +1415,15 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="135">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1436,15 +1432,15 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="120">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1453,15 +1449,15 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="120">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1470,15 +1466,15 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="120">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1487,15 +1483,15 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="120">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1504,12 +1500,12 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="6"/>
@@ -1517,15 +1513,15 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="45">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1534,15 +1530,15 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="45">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1551,35 +1547,37 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="90">
       <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="90">
       <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="C18" s="8" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="9" t="s">
@@ -1587,64 +1585,62 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45">
       <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="8" t="s">
+    <row r="20" spans="1:7" ht="30">
+      <c r="A20" s="11">
+        <v>2</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" ht="120">
+      <c r="A21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="345">
+      <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>2</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1653,15 +1649,15 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="30">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1670,15 +1666,15 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1687,15 +1683,15 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30">
       <c r="A25" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1704,15 +1700,15 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="C26" s="8" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1721,15 +1717,15 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="45">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1738,15 +1734,15 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="45">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1755,15 +1751,15 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="30">
       <c r="A29" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1772,15 +1768,15 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="30">
       <c r="A30" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1789,15 +1785,15 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="45">
       <c r="A31" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1806,15 +1802,15 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1823,45 +1819,45 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="8" t="s">
+    <row r="33" spans="1:7" ht="30">
+      <c r="A33" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" ht="45">
+      <c r="A34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C34" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="45">
+      <c r="A35" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="19"/>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="C35" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1870,15 +1866,15 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="60">
       <c r="A36" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1887,15 +1883,15 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="45">
       <c r="A37" s="3" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1904,15 +1900,15 @@
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="45">
       <c r="A38" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1921,15 +1917,15 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="45">
       <c r="A39" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1938,15 +1934,15 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="45">
       <c r="A40" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1955,15 +1951,15 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="60">
       <c r="A41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1972,15 +1968,15 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="45">
       <c r="A42" s="3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1989,15 +1985,15 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="45">
       <c r="A43" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2006,12 +2002,12 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="45">
       <c r="A44" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>107</v>
@@ -2023,15 +2019,15 @@
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="30">
       <c r="A45" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2040,59 +2036,42 @@
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="18"/>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A46" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="16"/>
+      <c r="F46" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="18"/>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2109,64 +2088,42 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="BLOCKED">
+  <conditionalFormatting sqref="F7:F13 F15:F19">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:F13">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH("BLOCKED",F8)))</formula>
+  <conditionalFormatting sqref="F21:F32">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F8)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",F8)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F20">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH("BLOCKED",F15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",F15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F33">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH("BLOCKED",F22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",F22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35:F47">
+  <conditionalFormatting sqref="F34:F46">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH("BLOCKED",F35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",F34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",F34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",F35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PASS",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F13 F15:F20 F22:F33 F35:F47">
-      <formula1>$A$317:$A$320</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:F32 F34:F46 F15:F19 F7:F13">
+      <formula1>$A$316:$A$319</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2175,142 +2132,142 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="27">
         <v>1</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="21">
         <f>COUNTIF(Sheet1!F7:F13, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="21">
         <f>COUNTIF(Sheet1!F7:F13, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="21">
         <f>COUNTIF(Sheet1!F7:F13, "NOT RUN")</f>
         <v>7</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="21">
         <f>COUNTIF(Sheet1!F7:F13, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+    <row r="9" spans="1:5">
+      <c r="A9" s="27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B9" s="33">
-        <f>COUNTIF(Sheet1!F15:F20, "PASS")</f>
+      <c r="B9" s="21">
+        <f>COUNTIF(Sheet1!F15:F19, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C9" s="33">
-        <f>COUNTIF(Sheet1!F15:F20, "FAIL")</f>
+      <c r="C9" s="21">
+        <f>COUNTIF(Sheet1!F15:F19, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D9" s="33">
-        <f>COUNTIF(Sheet1!F15:F20, "NOT RUN")</f>
-        <v>6</v>
-      </c>
-      <c r="E9" s="33">
-        <f>COUNTIF(Sheet1!F15:F20, "BLOCKED")</f>
+      <c r="D9" s="21">
+        <f>COUNTIF(Sheet1!F15:F19, "NOT RUN")</f>
+        <v>5</v>
+      </c>
+      <c r="E9" s="21">
+        <f>COUNTIF(Sheet1!F15:F19, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+    <row r="10" spans="1:5">
+      <c r="A10" s="27">
         <v>2</v>
       </c>
-      <c r="B10" s="33">
-        <f>COUNTIF(Sheet1!F22:F33, "PASS")</f>
+      <c r="B10" s="21">
+        <f>COUNTIF(Sheet1!F21:F32, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C10" s="33">
-        <f>COUNTIF(Sheet1!F22:F33, "FAIL")</f>
+      <c r="C10" s="21">
+        <f>COUNTIF(Sheet1!F21:F32, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D10" s="33">
-        <f>COUNTIF(Sheet1!F22:F33, "NOT RUN")</f>
+      <c r="D10" s="21">
+        <f>COUNTIF(Sheet1!F21:F32, "NOT RUN")</f>
         <v>12</v>
       </c>
-      <c r="E10" s="33">
-        <f>COUNTIF(Sheet1!F22:F33, "BLOCKED")</f>
+      <c r="E10" s="21">
+        <f>COUNTIF(Sheet1!F21:F32, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+    <row r="11" spans="1:5">
+      <c r="A11" s="27">
         <v>2.1</v>
       </c>
-      <c r="B11" s="33">
-        <f>COUNTIF(Sheet1!F35:F47, "PASS")</f>
+      <c r="B11" s="21">
+        <f>COUNTIF(Sheet1!F34:F46, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C11" s="33">
-        <f>COUNTIF(Sheet1!F35:F47, "FAIL")</f>
+      <c r="C11" s="21">
+        <f>COUNTIF(Sheet1!F34:F46, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D11" s="33">
-        <f>COUNTIF(Sheet1!F35:F47, "NOT RUN")</f>
+      <c r="D11" s="21">
+        <f>COUNTIF(Sheet1!F34:F46, "NOT RUN")</f>
         <v>13</v>
       </c>
-      <c r="E11" s="33">
-        <f>COUNTIF(Sheet1!F35:F47, "BLOCKED")</f>
+      <c r="E11" s="21">
+        <f>COUNTIF(Sheet1!F34:F46, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B12">
         <f>SUM(B8:B11)</f>
@@ -2322,7 +2279,7 @@
       </c>
       <c r="D12">
         <f>SUM(D8:D11)</f>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <f>SUM(E8:E11)</f>
@@ -2335,31 +2292,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Updated Test Cases for Log In
</commit_message>
<xml_diff>
--- a/documentation/quality/Test Documents/01 TC - Log In.Index.xlsx
+++ b/documentation/quality/Test Documents/01 TC - Log In.Index.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HostedRBI\apc-softdev-it111-06\documentation\quality\Test Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="19440" windowHeight="8010"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -503,8 +508,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,6 +871,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -913,7 +921,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -945,9 +953,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -979,6 +988,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1154,14 +1164,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -1172,7 +1182,7 @@
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>69</v>
       </c>
@@ -1183,7 +1193,7 @@
       <c r="F1" s="44"/>
       <c r="G1" s="45"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1219,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
@@ -1220,27 +1230,27 @@
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
       <c r="I3" s="46">
-        <f>AVERAGE(Sheet2!B12/38)</f>
+        <f>AVERAGE(Sheet2!B12/24)</f>
         <v>0</v>
       </c>
       <c r="J3" s="46">
-        <f>AVERAGE(Sheet2!C12/38)</f>
+        <f>AVERAGE(Sheet2!C12/24)</f>
         <v>0</v>
       </c>
       <c r="K3" s="46">
-        <f>AVERAGE(Sheet2!D12/38)</f>
-        <v>0.63157894736842102</v>
+        <f>AVERAGE(Sheet2!D12/24)</f>
+        <v>1</v>
       </c>
       <c r="L3" s="46">
-        <f>AVERAGE(Sheet2!E12/38)</f>
+        <f>AVERAGE(Sheet2!E12/24)</f>
         <v>0</v>
       </c>
       <c r="M3" s="46">
         <f>SUM(I3:L4)</f>
-        <v>0.63157894736842102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>70</v>
       </c>
@@ -1256,7 +1266,7 @@
       <c r="L4" s="46"/>
       <c r="M4" s="46"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>1</v>
       </c>
@@ -1269,7 +1279,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>2</v>
       </c>
@@ -1292,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="210.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:15" ht="210.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1328,7 @@
       <c r="N7" s="35"/>
       <c r="O7" s="36"/>
     </row>
-    <row r="8" spans="1:15" ht="90">
+    <row r="8" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1335,7 +1345,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="135">
+    <row r="9" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1352,7 +1362,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="120">
+    <row r="10" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1369,7 +1379,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="120">
+    <row r="11" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1386,7 +1396,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="120">
+    <row r="12" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1403,7 +1413,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="120">
+    <row r="13" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1420,7 +1430,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -1433,7 +1443,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="45">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1450,7 +1460,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="45">
+    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -1467,7 +1477,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="90">
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1486,7 +1496,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="90">
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1505,7 +1515,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="45">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1522,7 +1532,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="30">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>2</v>
       </c>
@@ -1535,7 +1545,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="225">
+    <row r="21" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
@@ -1552,7 +1562,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="75">
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
@@ -1569,7 +1579,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="60">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1586,7 +1596,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="90">
+    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1603,7 +1613,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="75">
+    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
@@ -1620,7 +1630,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="75">
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
@@ -1637,7 +1647,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>2.1</v>
       </c>
@@ -1650,7 +1660,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="19"/>
     </row>
-    <row r="28" spans="1:7" ht="45">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
@@ -1667,7 +1677,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -1684,7 +1694,7 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="60">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
@@ -1701,7 +1711,7 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="45">
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
@@ -1718,7 +1728,7 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="60">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>59</v>
       </c>
@@ -1735,7 +1745,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="45.75" thickBot="1">
+    <row r="33" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>60</v>
       </c>
@@ -1754,22 +1764,22 @@
       </c>
       <c r="G33" s="18"/>
     </row>
-    <row r="303" spans="1:1">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="304" spans="1:1">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="305" spans="1:1">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="1:1">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>10</v>
       </c>
@@ -1809,39 +1819,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>1</v>
       </c>
@@ -1879,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>1.1000000000000001</v>
       </c>
@@ -1900,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>2</v>
       </c>
@@ -1921,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>2.1</v>
       </c>
@@ -1942,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -1969,31 +1979,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>